<commit_message>
Added report for 3rd task
</commit_message>
<xml_diff>
--- a/Reports/Documents/Sprawozdanie3/Sprawozdanie3_WykresGantta.xlsx
+++ b/Reports/Documents/Sprawozdanie3/Sprawozdanie3_WykresGantta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nauka\Git\TPD\Reports\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nauka\Git\TPD\Reports\Documents\Sprawozdanie3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFE1324-2AF9-4AF3-BF0B-E1E033379CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706D23D7-2E27-4426-984B-B9F8EE645486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="1" xr2:uid="{C15BC6CE-4724-45C7-99E2-C70DD8428613}"/>
   </bookViews>
@@ -191,7 +191,11 @@
             <c:v>Początek</c:v>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -398,7 +402,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="90"/>
+        <c:gapWidth val="100"/>
         <c:overlap val="100"/>
         <c:axId val="243519984"/>
         <c:axId val="248663808"/>
@@ -432,16 +436,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
@@ -459,9 +463,8 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="23"/>
-          <c:min val="0"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
@@ -477,10 +480,37 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="d/mm;@" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="243519984"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
@@ -1459,17 +1489,16 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="12.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1480,7 +1509,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
@@ -1491,7 +1520,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
@@ -1502,7 +1531,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1">
@@ -1514,7 +1543,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
@@ -1526,7 +1555,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
@@ -1538,7 +1567,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
@@ -1550,7 +1579,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1">
@@ -1562,7 +1591,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1">
@@ -1574,7 +1603,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1">
@@ -1586,7 +1615,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1">

</xml_diff>